<commit_message>
Update data package at: 2024-08-06T19:17:53Z
</commit_message>
<xml_diff>
--- a/data-raw/aux-agrupamento-dcmefo.xlsx
+++ b/data-raw/aux-agrupamento-dcmefo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27813"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27930"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cecad365.sharepoint.com/sites/Splor/Documentos Compartilhados/General/@dcmefo/projetos/aux-agrupamento-dcmefo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_DAD87D3ED6CA80860BDB5A224BFFE83AD33AF163" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7396DD9-DE3D-4794-8FF0-88EEF0D169F3}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="11_DAD87D3ED6CA80860BDB5A224BFFE83AD33AF163" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6789946-4E6D-4489-8B24-4B24F7D10AB2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1649,14 +1649,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6743"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A501" workbookViewId="0">
-      <selection activeCell="D510" sqref="D510"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2028" sqref="A2028"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" customWidth="1"/>
     <col min="4" max="4" width="66" customWidth="1"/>
   </cols>
   <sheetData>
@@ -96063,20 +96063,12 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D6743" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B08D58FADB61F04EBBB4F355C06EFBED" ma:contentTypeVersion="18" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="1b889f39a240c2e855286b20cf95d05e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f4338ef-addb-4c87-aefe-1895241b335f" xmlns:ns3="b91e7f20-fe0a-487d-91a9-605ac1c64acf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="902f44b668f40cdc6ccc2fe791adf365" ns2:_="" ns3:_="">
     <xsd:import namespace="6f4338ef-addb-4c87-aefe-1895241b335f"/>
@@ -96331,10 +96323,19 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22B80336-12E8-4309-AF88-85CD791A8CDB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C1C34C7-C004-4355-8059-CB2E61C496EA}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C1C34C7-C004-4355-8059-CB2E61C496EA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22B80336-12E8-4309-AF88-85CD791A8CDB}"/>
 </file>
</xml_diff>